<commit_message>
ETHICS grades quiz 3
</commit_message>
<xml_diff>
--- a/1.1-CS-3162.052/Grades.xlsx
+++ b/1.1-CS-3162.052/Grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\UTDSpring2019\1.1-CS-3162.052\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142D4D61-E233-4449-B6E4-778C5C12A273}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7FBB6F-1B26-4A72-9FE2-722C95C1FEB6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4830" windowWidth="28755" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -675,7 +675,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="F7" s="9">
         <f t="shared" si="1"/>
-        <v>0.29625000000000001</v>
+        <v>0.28125</v>
       </c>
       <c r="G7" s="9">
         <f t="shared" si="1"/>
@@ -818,7 +818,7 @@
       <c r="I7" s="21"/>
       <c r="J7" s="21">
         <f>SUM(C7:H7)</f>
-        <v>0.99624999999999997</v>
+        <v>0.98124999999999996</v>
       </c>
       <c r="K7" s="21"/>
       <c r="L7" s="5"/>
@@ -861,7 +861,7 @@
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="19">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
@@ -882,7 +882,7 @@
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="19">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>

</xml_diff>

<commit_message>
ECS HW2 and grade for quiz 4
</commit_message>
<xml_diff>
--- a/1.1-CS-3162.052/Grades.xlsx
+++ b/1.1-CS-3162.052/Grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\UTDSpring2019\1.1-CS-3162.052\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7FBB6F-1B26-4A72-9FE2-722C95C1FEB6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADB6AAA-BF88-43A5-BEA2-3081EBB64EB5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4830" windowWidth="28755" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -675,7 +675,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +805,7 @@
       </c>
       <c r="F7" s="9">
         <f t="shared" si="1"/>
-        <v>0.28125</v>
+        <v>0.27374999999999999</v>
       </c>
       <c r="G7" s="9">
         <f t="shared" si="1"/>
@@ -818,7 +818,7 @@
       <c r="I7" s="21"/>
       <c r="J7" s="21">
         <f>SUM(C7:H7)</f>
-        <v>0.98124999999999996</v>
+        <v>0.97374999999999989</v>
       </c>
       <c r="K7" s="21"/>
       <c r="L7" s="5"/>
@@ -903,7 +903,7 @@
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="19">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>

</xml_diff>

<commit_message>
grades and budget update
</commit_message>
<xml_diff>
--- a/1.1-CS-3162.052/Grades.xlsx
+++ b/1.1-CS-3162.052/Grades.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\UTDSpring2019\1.1-CS-3162.052\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEEC267-503D-417D-9A10-CA32192C09CF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6795" yWindow="2580" windowWidth="21165" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6795" yWindow="3180" windowWidth="21165" windowHeight="12780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -77,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -427,23 +426,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -479,23 +461,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -671,11 +636,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,11 +762,11 @@
       </c>
       <c r="D7" s="9">
         <f t="shared" si="1"/>
-        <v>0.255</v>
+        <v>0.26250000000000001</v>
       </c>
       <c r="E7" s="9">
         <f t="shared" si="1"/>
-        <v>0.3</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F7" s="9">
         <f t="shared" si="1"/>
@@ -818,7 +783,7 @@
       <c r="I7" s="21"/>
       <c r="J7" s="21">
         <f>SUM(C7:H7)</f>
-        <v>0.91199999999999992</v>
+        <v>0.90449999999999997</v>
       </c>
       <c r="K7" s="21"/>
       <c r="L7" s="5"/>
@@ -837,7 +802,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="10">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="F8" s="18">
         <v>0.9</v>
@@ -899,7 +864,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="17">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="19">
@@ -1133,7 +1098,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1145,7 +1110,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Final debate turned in
</commit_message>
<xml_diff>
--- a/1.1-CS-3162.052/Grades.xlsx
+++ b/1.1-CS-3162.052/Grades.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\UTDSpring2019\1.1-CS-3162.052\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007B0A63-B169-41FD-B0CD-DFCDE10D3ACC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6795" yWindow="3180" windowWidth="21165" windowHeight="12780"/>
+    <workbookView xWindow="4455" yWindow="435" windowWidth="24345" windowHeight="10635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -76,7 +77,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -426,6 +427,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -461,6 +479,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -636,11 +671,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,11 +797,11 @@
       </c>
       <c r="D7" s="9">
         <f t="shared" si="1"/>
-        <v>0.26250000000000001</v>
+        <v>0.27750000000000002</v>
       </c>
       <c r="E7" s="9">
         <f t="shared" si="1"/>
-        <v>0.28499999999999998</v>
+        <v>0.27750000000000002</v>
       </c>
       <c r="F7" s="9">
         <f t="shared" si="1"/>
@@ -783,7 +818,7 @@
       <c r="I7" s="21"/>
       <c r="J7" s="21">
         <f>SUM(C7:H7)</f>
-        <v>0.90449999999999997</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="K7" s="21"/>
       <c r="L7" s="5"/>
@@ -802,7 +837,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="10">
-        <v>0.95</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="F8" s="18">
         <v>0.9</v>
@@ -822,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="17">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="19">
@@ -1098,7 +1133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1110,7 +1145,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>